<commit_message>
Added link to readme.md
</commit_message>
<xml_diff>
--- a/php_translation_helper.xlsx
+++ b/php_translation_helper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\Prj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Dev\0020_Web\0005_Kanboard\20_php_Translation_Helper\php_Translation_Helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="21900" windowHeight="11130"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="21900" windowHeight="11130"/>
   </bookViews>
   <sheets>
     <sheet name="Fileconverter" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>&lt;?php</t>
   </si>
@@ -157,12 +157,41 @@
   <si>
     <t>3. copy here the translation from deepl.com (target language)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>readme.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for more information:</t>
+    </r>
+  </si>
+  <si>
+    <t>readme.md on GitHub</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +249,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -244,10 +281,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,12 +304,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -279,8 +320,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -301,10 +345,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -319,23 +359,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B9:D100" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B10:D101" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="3">
-    <tableColumn id="5" name="1. copy only the text file rows here from the source file" dataDxfId="3"/>
-    <tableColumn id="1" name="2. automatic text extract of source file" dataDxfId="2">
-      <calculatedColumnFormula>IF(B10&lt;&gt;"",MID(B10,FIND("'",B10)+1,FIND("'",B10,FIND("'",B10)+1)-FIND("'",B10)-1),"")</calculatedColumnFormula>
+    <tableColumn id="5" name="1. copy only the text file rows here from the source file" dataDxfId="6"/>
+    <tableColumn id="1" name="2. automatic text extract of source file" dataDxfId="5">
+      <calculatedColumnFormula>IF(B11&lt;&gt;"",MID(B11,FIND("'",B11)+1,FIND("'",B11,FIND("'",B11)+1)-FIND("'",B11)-1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="3. copy here the translation from deepl.com (target language)" dataDxfId="1"/>
+    <tableColumn id="2" name="3. copy here the translation from deepl.com (target language)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle13" displayName="Tabelle13" ref="B9:C100" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle13" displayName="Tabelle13" ref="B9:C100" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" name="1. type or copy your source texts here" dataDxfId="5"/>
-    <tableColumn id="2" name="2. copy here the translation from deepl.com (target language)" dataDxfId="4"/>
+    <tableColumn id="1" name="1. type or copy your source texts here" dataDxfId="1"/>
+    <tableColumn id="2" name="2. copy here the translation from deepl.com (target language)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,9 +647,11 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:E100"/>
+  <dimension ref="B2:E101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -632,7 +674,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -642,1131 +684,1141 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="10"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="E9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="5" t="str">
-        <f>IF(B10&lt;&gt;"",MID(B10,FIND("'",B10)+1,FIND("'",B10,FIND("'",B10)+1)-FIND("'",B10)-1),"")</f>
-        <v/>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3" t="str">
-        <f>IF(C10&lt;&gt;"",CHAR(39)&amp;C10&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D10&amp;CHAR(39)&amp;",",IF(AND(E9&lt;&gt;"",E9&lt;&gt;");"),");",""))</f>
-        <v>);</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="5" t="str">
-        <f t="shared" ref="C11:C39" si="0">IF(B11&lt;&gt;"",MID(B11,FIND("'",B11)+1,FIND("'",B11,FIND("'",B11)+1)-FIND("'",B11)-1),"")</f>
-        <v/>
-      </c>
-      <c r="D11" s="5"/>
+        <f>IF(B11&lt;&gt;"",MID(B11,FIND("'",B11)+1,FIND("'",B11,FIND("'",B11)+1)-FIND("'",B11)-1),"")</f>
+        <v/>
+      </c>
+      <c r="D11" s="6"/>
       <c r="E11" s="3" t="str">
-        <f>IF(C11&lt;&gt;"",CHAR(39)&amp;C11&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D11&amp;CHAR(39)&amp;",",IF(AND(E10&lt;&gt;"",E10&lt;&gt;");"),");",""))</f>
-        <v/>
+        <f t="shared" ref="E11:E40" si="0">IF(C11&lt;&gt;"",CHAR(39)&amp;C11&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D11&amp;CHAR(39)&amp;",",IF(AND(E10&lt;&gt;"",E10&lt;&gt;");"),");",""))</f>
+        <v>);</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C12:C40" si="1">IF(B12&lt;&gt;"",MID(B12,FIND("'",B12)+1,FIND("'",B12,FIND("'",B12)+1)-FIND("'",B12)-1),"")</f>
         <v/>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="str">
-        <f>IF(C12&lt;&gt;"",CHAR(39)&amp;C12&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D12&amp;CHAR(39)&amp;",",IF(AND(E11&lt;&gt;"",E11&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="str">
-        <f>IF(C13&lt;&gt;"",CHAR(39)&amp;C13&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D13&amp;CHAR(39)&amp;",",IF(AND(E12&lt;&gt;"",E12&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="3" t="str">
-        <f>IF(C14&lt;&gt;"",CHAR(39)&amp;C14&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D14&amp;CHAR(39)&amp;",",IF(AND(E13&lt;&gt;"",E13&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="str">
-        <f>IF(C15&lt;&gt;"",CHAR(39)&amp;C15&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D15&amp;CHAR(39)&amp;",",IF(AND(E14&lt;&gt;"",E14&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3" t="str">
-        <f>IF(C16&lt;&gt;"",CHAR(39)&amp;C16&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D16&amp;CHAR(39)&amp;",",IF(AND(E15&lt;&gt;"",E15&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="3" t="str">
-        <f>IF(C17&lt;&gt;"",CHAR(39)&amp;C17&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D17&amp;CHAR(39)&amp;",",IF(AND(E16&lt;&gt;"",E16&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="3" t="str">
-        <f>IF(C18&lt;&gt;"",CHAR(39)&amp;C18&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D18&amp;CHAR(39)&amp;",",IF(AND(E17&lt;&gt;"",E17&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3" t="str">
-        <f>IF(C19&lt;&gt;"",CHAR(39)&amp;C19&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D19&amp;CHAR(39)&amp;",",IF(AND(E18&lt;&gt;"",E18&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3" t="str">
-        <f>IF(C20&lt;&gt;"",CHAR(39)&amp;C20&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D20&amp;CHAR(39)&amp;",",IF(AND(E19&lt;&gt;"",E19&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3" t="str">
-        <f>IF(C21&lt;&gt;"",CHAR(39)&amp;C21&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D21&amp;CHAR(39)&amp;",",IF(AND(E20&lt;&gt;"",E20&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3" t="str">
-        <f>IF(C22&lt;&gt;"",CHAR(39)&amp;C22&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D22&amp;CHAR(39)&amp;",",IF(AND(E21&lt;&gt;"",E21&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="3" t="str">
-        <f>IF(C23&lt;&gt;"",CHAR(39)&amp;C23&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D23&amp;CHAR(39)&amp;",",IF(AND(E22&lt;&gt;"",E22&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="3" t="str">
-        <f>IF(C24&lt;&gt;"",CHAR(39)&amp;C24&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D24&amp;CHAR(39)&amp;",",IF(AND(E23&lt;&gt;"",E23&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="3" t="str">
-        <f>IF(C25&lt;&gt;"",CHAR(39)&amp;C25&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D25&amp;CHAR(39)&amp;",",IF(AND(E24&lt;&gt;"",E24&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="3" t="str">
-        <f>IF(C26&lt;&gt;"",CHAR(39)&amp;C26&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D26&amp;CHAR(39)&amp;",",IF(AND(E25&lt;&gt;"",E25&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="3" t="str">
-        <f>IF(C27&lt;&gt;"",CHAR(39)&amp;C27&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D27&amp;CHAR(39)&amp;",",IF(AND(E26&lt;&gt;"",E26&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="3" t="str">
-        <f>IF(C28&lt;&gt;"",CHAR(39)&amp;C28&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D28&amp;CHAR(39)&amp;",",IF(AND(E27&lt;&gt;"",E27&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="3" t="str">
-        <f>IF(C29&lt;&gt;"",CHAR(39)&amp;C29&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D29&amp;CHAR(39)&amp;",",IF(AND(E28&lt;&gt;"",E28&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D30" s="6"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="3" t="str">
-        <f>IF(C30&lt;&gt;"",CHAR(39)&amp;C30&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D30&amp;CHAR(39)&amp;",",IF(AND(E29&lt;&gt;"",E29&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="3" t="str">
-        <f>IF(C31&lt;&gt;"",CHAR(39)&amp;C31&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D31&amp;CHAR(39)&amp;",",IF(AND(E30&lt;&gt;"",E30&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="3" t="str">
-        <f>IF(C32&lt;&gt;"",CHAR(39)&amp;C32&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D32&amp;CHAR(39)&amp;",",IF(AND(E31&lt;&gt;"",E31&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="3" t="str">
-        <f>IF(C33&lt;&gt;"",CHAR(39)&amp;C33&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D33&amp;CHAR(39)&amp;",",IF(AND(E32&lt;&gt;"",E32&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="3" t="str">
-        <f>IF(C34&lt;&gt;"",CHAR(39)&amp;C34&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D34&amp;CHAR(39)&amp;",",IF(AND(E33&lt;&gt;"",E33&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="3" t="str">
-        <f>IF(C35&lt;&gt;"",CHAR(39)&amp;C35&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D35&amp;CHAR(39)&amp;",",IF(AND(E34&lt;&gt;"",E34&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="3" t="str">
-        <f>IF(C36&lt;&gt;"",CHAR(39)&amp;C36&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D36&amp;CHAR(39)&amp;",",IF(AND(E35&lt;&gt;"",E35&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="C37" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="3" t="str">
-        <f>IF(C37&lt;&gt;"",CHAR(39)&amp;C37&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D37&amp;CHAR(39)&amp;",",IF(AND(E36&lt;&gt;"",E36&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="3" t="str">
-        <f>IF(C38&lt;&gt;"",CHAR(39)&amp;C38&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D38&amp;CHAR(39)&amp;",",IF(AND(E37&lt;&gt;"",E37&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="3" t="str">
-        <f>IF(C39&lt;&gt;"",CHAR(39)&amp;C39&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D39&amp;CHAR(39)&amp;",",IF(AND(E38&lt;&gt;"",E38&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
-      <c r="C40" s="6" t="str">
-        <f t="shared" ref="C40:C71" si="1">IF(B40&lt;&gt;"",MID(B40,FIND("'",B40)+1,FIND("'",B40,FIND("'",B40)+1)-FIND("'",B40)-1),"")</f>
+      <c r="C40" s="5" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="3" t="str">
-        <f t="shared" ref="E40:E100" si="2">IF(C40&lt;&gt;"",CHAR(39)&amp;C40&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D40&amp;CHAR(39)&amp;",",IF(AND(E39&lt;&gt;"",E39&lt;&gt;");"),");",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C41:C72" si="2">IF(B41&lt;&gt;"",MID(B41,FIND("'",B41)+1,FIND("'",B41,FIND("'",B41)+1)-FIND("'",B41)-1),"")</f>
         <v/>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E41:E101" si="3">IF(C41&lt;&gt;"",CHAR(39)&amp;C41&amp;CHAR(39)&amp;"  =&gt;  "&amp;CHAR(39)&amp;D41&amp;CHAR(39)&amp;",",IF(AND(E40&lt;&gt;"",E40&lt;&gt;");"),");",""))</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="C49" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="str">
-        <f t="shared" ref="C72:C103" si="3">IF(B72&lt;&gt;"",MID(B72,FIND("'",B72)+1,FIND("'",B72,FIND("'",B72)+1)-FIND("'",B72)-1),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C73:C101" si="4">IF(B73&lt;&gt;"",MID(B73,FIND("'",B73)+1,FIND("'",B73,FIND("'",B73)+1)-FIND("'",B73)-1),"")</f>
         <v/>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="C82" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="C83" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="C85" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="C86" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="C87" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
       <c r="C93" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
       <c r="C94" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="C95" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
       <c r="C96" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D96" s="6"/>
       <c r="E96" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
       <c r="C97" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D98" s="6"/>
       <c r="E98" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D99" s="6"/>
       <c r="E99" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
       <c r="C100" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="6"/>
+      <c r="C101" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D101" s="6"/>
+      <c r="E101" s="3" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>